<commit_message>
added cross-temporal reconciliation using FoReco
</commit_message>
<xml_diff>
--- a/Accuracy_New.xlsx
+++ b/Accuracy_New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00c848d2da39f20/Documents/3. Masters/Research/WindPowerForecasting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{8A1A52A6-25A9-4C60-9B01-BC522629704C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42D2057C-0F61-4A9C-B567-3D5D7029FD49}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{8A1A52A6-25A9-4C60-9B01-BC522629704C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7586539-6325-474F-8750-6FDD98EF22C9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{82814EFC-B74C-4BDB-8AD7-326D4ADF3E3A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="20">
   <si>
     <t>Level</t>
   </si>
@@ -94,6 +94,9 @@
   <si>
     <t>`</t>
   </si>
+  <si>
+    <t>20-Minutely</t>
+  </si>
 </sst>
 </file>
 
@@ -137,267 +140,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -891,12 +634,12 @@
   <dimension ref="A1:Q49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+      <selection activeCell="K24" sqref="K24:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -909,8 +652,14 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -936,7 +685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -955,8 +704,14 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H3">
+        <v>0.59262992211717402</v>
+      </c>
+      <c r="I3">
+        <v>0.59228988890613399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -975,8 +730,14 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H4">
+        <v>0.61696749954032803</v>
+      </c>
+      <c r="I4">
+        <v>0.58440422131718694</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -995,8 +756,14 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H5">
+        <v>0.58439289358906499</v>
+      </c>
+      <c r="I5">
+        <v>0.56664287382535605</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1015,8 +782,14 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H6">
+        <v>0.601432686063892</v>
+      </c>
+      <c r="I6">
+        <v>0.57496097891783604</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1035,8 +808,14 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H7">
+        <v>0.58587958949003904</v>
+      </c>
+      <c r="I7">
+        <v>0.56736743707290604</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1055,8 +834,14 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H8">
+        <v>0.58205254989342103</v>
+      </c>
+      <c r="I8">
+        <v>0.56582760110948205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1075,8 +860,14 @@
       <c r="G9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H9">
+        <v>0.60991603673899697</v>
+      </c>
+      <c r="I9">
+        <v>0.57745330359948399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1095,8 +886,14 @@
       <c r="G10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H10">
+        <v>0.59017795164920805</v>
+      </c>
+      <c r="I10">
+        <v>0.57088853150605701</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1115,8 +912,14 @@
       <c r="G11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H11">
+        <v>0.59492656799399402</v>
+      </c>
+      <c r="I11">
+        <v>0.572034381899162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1135,8 +938,14 @@
       <c r="G12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H12">
+        <v>0.59054681313225998</v>
+      </c>
+      <c r="I12">
+        <v>0.57278103779853295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1155,8 +964,14 @@
       <c r="G13">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H13">
+        <v>0.59384605685680003</v>
+      </c>
+      <c r="I13">
+        <v>0.57657612060677399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1175,8 +990,14 @@
       <c r="G15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H15">
+        <v>0.62783724785218897</v>
+      </c>
+      <c r="I15">
+        <v>0.63281554158687103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1195,8 +1016,14 @@
       <c r="G16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16">
+        <v>0.64786641834776604</v>
+      </c>
+      <c r="I16">
+        <v>0.62148603620267495</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1215,8 +1042,14 @@
       <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17">
+        <v>0.62625190505823403</v>
+      </c>
+      <c r="I17">
+        <v>0.60774102857444401</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1235,8 +1068,14 @@
       <c r="G18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18">
+        <v>0.63925776169135995</v>
+      </c>
+      <c r="I18">
+        <v>0.61753511070994804</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1255,8 +1094,14 @@
       <c r="G19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19">
+        <v>0.62757255442682502</v>
+      </c>
+      <c r="I19">
+        <v>0.61159695233658895</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1275,8 +1120,14 @@
       <c r="G20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20">
+        <v>0.62529430647119799</v>
+      </c>
+      <c r="I20">
+        <v>0.61089907980883795</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1295,8 +1146,14 @@
       <c r="G21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21">
+        <v>0.64665288390991704</v>
+      </c>
+      <c r="I21">
+        <v>0.61875220356414595</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -1315,8 +1172,14 @@
       <c r="G22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22">
+        <v>0.63229164172187302</v>
+      </c>
+      <c r="I22">
+        <v>0.61399954913638699</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1335,8 +1198,14 @@
       <c r="G23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23">
+        <v>0.64362344157642304</v>
+      </c>
+      <c r="I23">
+        <v>0.62124119547498502</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1355,8 +1224,14 @@
       <c r="G24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24">
+        <v>0.64223177493422001</v>
+      </c>
+      <c r="I24">
+        <v>0.62289016755623805</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1375,8 +1250,14 @@
       <c r="G25">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25">
+        <v>0.64341329607339603</v>
+      </c>
+      <c r="I25">
+        <v>0.62499735838235104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1395,8 +1276,14 @@
       <c r="G27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27">
+        <v>0.63510687410187805</v>
+      </c>
+      <c r="I27">
+        <v>0.64684753179853105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -1415,8 +1302,14 @@
       <c r="G28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H28">
+        <v>0.65972461838747298</v>
+      </c>
+      <c r="I28">
+        <v>0.63391139708470001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1435,8 +1328,14 @@
       <c r="G29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29">
+        <v>0.64090085114085305</v>
+      </c>
+      <c r="I29">
+        <v>0.62273857244063402</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1455,8 +1354,14 @@
       <c r="G30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30">
+        <v>0.651732508098115</v>
+      </c>
+      <c r="I30">
+        <v>0.63031154957941404</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1475,8 +1380,14 @@
       <c r="G31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31">
+        <v>0.642878314447483</v>
+      </c>
+      <c r="I31">
+        <v>0.62598258905808901</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1494,6 +1405,12 @@
       </c>
       <c r="G32">
         <v>2</v>
+      </c>
+      <c r="H32">
+        <v>0.64020151108549594</v>
+      </c>
+      <c r="I32">
+        <v>0.62511054824894297</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">
@@ -1515,6 +1432,12 @@
       <c r="G33">
         <v>2</v>
       </c>
+      <c r="H33">
+        <v>0.66675927169618199</v>
+      </c>
+      <c r="I33">
+        <v>0.63677484968313702</v>
+      </c>
       <c r="Q33" t="s">
         <v>18</v>
       </c>
@@ -1538,6 +1461,12 @@
       <c r="G34">
         <v>2</v>
       </c>
+      <c r="H34">
+        <v>0.65520537905050702</v>
+      </c>
+      <c r="I34">
+        <v>0.63306288024300506</v>
+      </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
@@ -1558,6 +1487,12 @@
       <c r="G35">
         <v>2</v>
       </c>
+      <c r="H35">
+        <v>0.66471492548870803</v>
+      </c>
+      <c r="I35">
+        <v>0.63859731153465804</v>
+      </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
@@ -1578,6 +1513,12 @@
       <c r="G36">
         <v>2</v>
       </c>
+      <c r="H36">
+        <v>0.66105660779304098</v>
+      </c>
+      <c r="I36">
+        <v>0.63834629950968103</v>
+      </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -1598,6 +1539,12 @@
       <c r="G37">
         <v>2</v>
       </c>
+      <c r="H37">
+        <v>0.6643183461769</v>
+      </c>
+      <c r="I37">
+        <v>0.64172934138187399</v>
+      </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
@@ -1620,6 +1567,14 @@
       <c r="G39" t="s">
         <v>15</v>
       </c>
+      <c r="H39">
+        <f>AVERAGE(H27,H15,H3)</f>
+        <v>0.61852468135708027</v>
+      </c>
+      <c r="I39">
+        <f>AVERAGE(I27,I15,I3)</f>
+        <v>0.62398432076384536</v>
+      </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
@@ -1642,6 +1597,14 @@
       <c r="G40" t="s">
         <v>15</v>
       </c>
+      <c r="H40">
+        <f t="shared" ref="H40:I40" si="1">AVERAGE(H28,H16,H4)</f>
+        <v>0.64151951209185565</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>0.61326721820152064</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
@@ -1664,6 +1627,14 @@
       <c r="G41" t="s">
         <v>15</v>
       </c>
+      <c r="H41">
+        <f t="shared" ref="H41:I41" si="2">AVERAGE(H29,H17,H5)</f>
+        <v>0.61718188326271739</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="2"/>
+        <v>0.59904082494681132</v>
+      </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
@@ -1686,6 +1657,14 @@
       <c r="G42" t="s">
         <v>15</v>
       </c>
+      <c r="H42">
+        <f t="shared" ref="H42:I42" si="3">AVERAGE(H30,H18,H6)</f>
+        <v>0.63080765195112232</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="3"/>
+        <v>0.60760254640239941</v>
+      </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
@@ -1708,6 +1687,14 @@
       <c r="G43" t="s">
         <v>15</v>
       </c>
+      <c r="H43">
+        <f t="shared" ref="H43:I43" si="4">AVERAGE(H31,H19,H7)</f>
+        <v>0.61877681945478236</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="4"/>
+        <v>0.60164899282252804</v>
+      </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
@@ -1730,6 +1717,14 @@
       <c r="G44" t="s">
         <v>15</v>
       </c>
+      <c r="H44">
+        <f t="shared" ref="H44:I44" si="5">AVERAGE(H32,H20,H8)</f>
+        <v>0.61584945581670503</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="5"/>
+        <v>0.60061240972242103</v>
+      </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
@@ -1752,6 +1747,14 @@
       <c r="G45" t="s">
         <v>15</v>
       </c>
+      <c r="H45">
+        <f t="shared" ref="H45:I45" si="6">AVERAGE(H33,H21,H9)</f>
+        <v>0.64110939744836537</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="6"/>
+        <v>0.61099345228225566</v>
+      </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
@@ -1774,6 +1777,14 @@
       <c r="G46" t="s">
         <v>15</v>
       </c>
+      <c r="H46">
+        <f t="shared" ref="H46:I46" si="7">AVERAGE(H34,H22,H10)</f>
+        <v>0.62589165747386266</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="7"/>
+        <v>0.60598365362848305</v>
+      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
@@ -1796,6 +1807,14 @@
       <c r="G47" t="s">
         <v>15</v>
       </c>
+      <c r="H47">
+        <f t="shared" ref="H47:I47" si="8">AVERAGE(H35,H23,H11)</f>
+        <v>0.63442164501970844</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="8"/>
+        <v>0.61062429630293502</v>
+      </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
@@ -1818,8 +1837,16 @@
       <c r="G48" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H48">
+        <f t="shared" ref="H48:I48" si="9">AVERAGE(H36,H24,H12)</f>
+        <v>0.63127839861984036</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="9"/>
+        <v>0.61133916828815071</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>14</v>
       </c>
@@ -1840,53 +1867,62 @@
       <c r="G49" t="s">
         <v>15</v>
       </c>
+      <c r="H49">
+        <f t="shared" ref="H49:I49" si="10">AVERAGE(H37,H25,H13)</f>
+        <v>0.63385923303569869</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="10"/>
+        <v>0.61443427345699975</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C13">
+    <cfRule type="top10" dxfId="17" priority="18" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D13">
+    <cfRule type="top10" dxfId="16" priority="17" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:C25">
     <cfRule type="top10" dxfId="15" priority="16" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D13">
+  <conditionalFormatting sqref="D15:D25">
     <cfRule type="top10" dxfId="14" priority="15" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C25">
+  <conditionalFormatting sqref="C27:C37">
     <cfRule type="top10" dxfId="13" priority="14" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15:D25">
+  <conditionalFormatting sqref="D27:D37">
     <cfRule type="top10" dxfId="12" priority="13" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:C37">
+  <conditionalFormatting sqref="C39:C49">
     <cfRule type="top10" dxfId="11" priority="12" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27:D37">
+  <conditionalFormatting sqref="D39:D49">
     <cfRule type="top10" dxfId="10" priority="11" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39:C49">
+  <conditionalFormatting sqref="H3:H13">
     <cfRule type="top10" dxfId="9" priority="10" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39:D49">
+  <conditionalFormatting sqref="I3:I13">
     <cfRule type="top10" dxfId="8" priority="9" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H13">
+  <conditionalFormatting sqref="H15 H21:H25">
     <cfRule type="top10" dxfId="7" priority="8" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I13">
+  <conditionalFormatting sqref="I15 I21:I25">
     <cfRule type="top10" dxfId="6" priority="7" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H15:H25">
+  <conditionalFormatting sqref="H27:H37">
     <cfRule type="top10" dxfId="5" priority="6" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15:I25">
+  <conditionalFormatting sqref="I27:I37">
     <cfRule type="top10" dxfId="4" priority="5" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27:H37">
-    <cfRule type="top10" dxfId="3" priority="4" bottom="1" rank="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I27:I37">
-    <cfRule type="top10" dxfId="2" priority="3" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39:H49">
     <cfRule type="top10" dxfId="1" priority="2" bottom="1" rank="1"/>

</xml_diff>